<commit_message>
update  module seeder create company seeder update company id on user details
</commit_message>
<xml_diff>
--- a/database/seeders/excel/user_niise_baru.xlsx
+++ b/database/seeders/excel/user_niise_baru.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\storage\app\private\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB63859-AC50-4BB3-A3D2-77DFBF01AC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8E5ABF-37B4-4C37-ACC7-F38364DA11D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9578E655-562C-4104-B8F7-418F8D65ADB7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="360">
   <si>
     <t>Jabatan Imigresen Malaysia Negeri Johor</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Pejabat Imigresen Pelabuhan Melaka (ICQS)</t>
   </si>
   <si>
-    <t>Jabatan Imigresen Negeri Melaka</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jabatan Imigresen Malaysia Negeri Sembilan </t>
   </si>
   <si>
@@ -119,14 +116,7 @@
     <t>Pejabat Imigresen Lapangan Terbang Antarabangsa Kuala Lumpur (KLIA)</t>
   </si>
   <si>
-    <t xml:space="preserve">Jabatan Imigresen Malaysia 
-Wilayah Persekutuan Kuala Lumpur, </t>
-  </si>
-  <si>
     <t xml:space="preserve">Depot Imigresen Bukit Jalil, </t>
-  </si>
-  <si>
-    <t>Jabatan Imigresen WP Kuala Lumpur</t>
   </si>
   <si>
     <t>Jabatan Imigresen Malaysia
@@ -1121,6 +1111,12 @@
   </si>
   <si>
     <t>nabilahs@heitech.com.my</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jabatan Imigresen Malaysia Wilayah Persekutuan Kuala Lumpur, </t>
+  </si>
+  <si>
+    <t>Jabatan Imigresen Malaysia Wilayah Persekutuan Kuala Lumpur</t>
   </si>
 </sst>
 </file>
@@ -1566,1862 +1562,1866 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C254406F-12FB-4ABC-BFDB-626D932D93E0}">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
     <col min="2" max="2" width="68.28515625" customWidth="1"/>
     <col min="3" max="3" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E29" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" t="s">
         <v>54</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" t="s">
-        <v>160</v>
-      </c>
-      <c r="E31" t="s">
-        <v>161</v>
-      </c>
-      <c r="F31" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E32" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E33" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34" t="s">
         <v>54</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" t="s">
-        <v>169</v>
-      </c>
-      <c r="E34" t="s">
-        <v>170</v>
-      </c>
-      <c r="F34" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E35" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E36" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E37" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E38" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E40" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" t="s">
+        <v>178</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" t="s">
         <v>180</v>
-      </c>
-      <c r="B41" t="s">
-        <v>181</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" t="s">
-        <v>182</v>
-      </c>
-      <c r="E41" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B42" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E42" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" t="s">
         <v>187</v>
       </c>
-      <c r="B43" t="s">
-        <v>188</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" t="s">
-        <v>189</v>
-      </c>
-      <c r="E43" t="s">
-        <v>190</v>
-      </c>
       <c r="F43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E44" t="s">
         <v>191</v>
-      </c>
-      <c r="B44" t="s">
-        <v>192</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" t="s">
-        <v>193</v>
-      </c>
-      <c r="E44" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E45" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E46" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F46" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>201</v>
+      </c>
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>202</v>
+      </c>
+      <c r="E48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>204</v>
       </c>
-      <c r="B48" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B49" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" t="s">
         <v>22</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>205</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="F49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>207</v>
       </c>
-      <c r="B49" t="s">
-        <v>188</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>208</v>
+      </c>
+      <c r="E50" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>210</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>211</v>
+      </c>
+      <c r="E51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>213</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
         <v>23</v>
       </c>
-      <c r="D49" t="s">
-        <v>208</v>
-      </c>
-      <c r="E49" t="s">
-        <v>209</v>
-      </c>
-      <c r="F49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>210</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="D52" t="s">
+        <v>214</v>
+      </c>
+      <c r="E52" t="s">
+        <v>215</v>
+      </c>
+      <c r="F52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>216</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" t="s">
         <v>23</v>
       </c>
-      <c r="D50" t="s">
-        <v>211</v>
-      </c>
-      <c r="E50" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>213</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D53" t="s">
+        <v>217</v>
+      </c>
+      <c r="E53" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>219</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" t="s">
         <v>23</v>
       </c>
-      <c r="D51" t="s">
-        <v>214</v>
-      </c>
-      <c r="E51" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>216</v>
-      </c>
-      <c r="B52" s="3" t="s">
+      <c r="D54" t="s">
+        <v>220</v>
+      </c>
+      <c r="E54" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>222</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" t="s">
+        <v>223</v>
+      </c>
+      <c r="F55" t="s">
         <v>54</v>
       </c>
-      <c r="C52" t="s">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>224</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s">
         <v>24</v>
       </c>
-      <c r="D52" t="s">
-        <v>217</v>
-      </c>
-      <c r="E52" t="s">
-        <v>218</v>
-      </c>
-      <c r="F52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>219</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D56" t="s">
+        <v>225</v>
+      </c>
+      <c r="E56" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>227</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" t="s">
         <v>24</v>
       </c>
-      <c r="D53" t="s">
-        <v>220</v>
-      </c>
-      <c r="E53" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>222</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" t="s">
-        <v>223</v>
-      </c>
-      <c r="E54" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>225</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D57" t="s">
+        <v>228</v>
+      </c>
+      <c r="E57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D55" t="s">
-        <v>226</v>
-      </c>
-      <c r="F55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>227</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D58" t="s">
+        <v>231</v>
+      </c>
+      <c r="F58" t="s">
+        <v>54</v>
+      </c>
+      <c r="J58" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D56" t="s">
-        <v>228</v>
-      </c>
-      <c r="E56" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>230</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D59" t="s">
+        <v>233</v>
+      </c>
+      <c r="E59" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>235</v>
+      </c>
+      <c r="B60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" t="s">
         <v>25</v>
       </c>
-      <c r="D57" t="s">
-        <v>231</v>
-      </c>
-      <c r="E57" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>233</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="D60" t="s">
+        <v>236</v>
+      </c>
+      <c r="E60" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>238</v>
+      </c>
+      <c r="B61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D61" t="s">
+        <v>239</v>
+      </c>
+      <c r="F61" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="1" t="s">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>240</v>
+      </c>
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
         <v>26</v>
       </c>
-      <c r="D58" t="s">
-        <v>234</v>
-      </c>
-      <c r="F58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>235</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" t="s">
-        <v>236</v>
-      </c>
-      <c r="E59" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>238</v>
-      </c>
-      <c r="B60" t="s">
-        <v>181</v>
-      </c>
-      <c r="C60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" t="s">
-        <v>239</v>
-      </c>
-      <c r="E60" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="F62" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>241</v>
       </c>
-      <c r="B61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" t="s">
-        <v>27</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B63" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" t="s">
+        <v>359</v>
+      </c>
+      <c r="D63" t="s">
         <v>242</v>
       </c>
-      <c r="F61" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="E63" t="s">
         <v>243</v>
       </c>
-      <c r="B62" t="s">
-        <v>129</v>
-      </c>
-      <c r="C62" t="s">
-        <v>28</v>
-      </c>
-      <c r="F62" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>244</v>
       </c>
-      <c r="B63" t="s">
-        <v>153</v>
-      </c>
-      <c r="C63" t="s">
-        <v>29</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B64" t="s">
+        <v>178</v>
+      </c>
+      <c r="C64" t="s">
+        <v>359</v>
+      </c>
+      <c r="D64" t="s">
         <v>245</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>247</v>
-      </c>
-      <c r="B64" t="s">
-        <v>181</v>
-      </c>
-      <c r="C64" t="s">
-        <v>29</v>
-      </c>
-      <c r="D64" t="s">
-        <v>248</v>
-      </c>
-      <c r="E64" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" t="s">
+        <v>248</v>
+      </c>
+      <c r="F65" t="s">
         <v>54</v>
-      </c>
-      <c r="C65" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" t="s">
-        <v>251</v>
-      </c>
-      <c r="F65" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B66" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E66" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C67" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D67" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E67" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>255</v>
+      </c>
+      <c r="B68" t="s">
+        <v>256</v>
+      </c>
+      <c r="C68" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" t="s">
+        <v>257</v>
+      </c>
+      <c r="E68" t="s">
         <v>258</v>
       </c>
-      <c r="B68" t="s">
+      <c r="F68" t="s">
         <v>259</v>
-      </c>
-      <c r="C68" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" t="s">
-        <v>260</v>
-      </c>
-      <c r="E68" t="s">
-        <v>261</v>
-      </c>
-      <c r="F68" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>260</v>
+      </c>
+      <c r="B69" t="s">
+        <v>261</v>
+      </c>
+      <c r="C69" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" t="s">
+        <v>262</v>
+      </c>
+      <c r="E69" t="s">
         <v>263</v>
       </c>
-      <c r="B69" t="s">
+      <c r="F69" t="s">
         <v>264</v>
-      </c>
-      <c r="C69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D69" t="s">
-        <v>265</v>
-      </c>
-      <c r="E69" t="s">
-        <v>266</v>
-      </c>
-      <c r="F69" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>265</v>
+      </c>
+      <c r="B70" t="s">
+        <v>266</v>
+      </c>
+      <c r="C70" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" t="s">
+        <v>267</v>
+      </c>
+      <c r="E70" t="s">
         <v>268</v>
       </c>
-      <c r="B70" t="s">
+      <c r="F70" t="s">
         <v>269</v>
-      </c>
-      <c r="C70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D70" t="s">
-        <v>270</v>
-      </c>
-      <c r="E70" t="s">
-        <v>271</v>
-      </c>
-      <c r="F70" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>270</v>
+      </c>
+      <c r="B71" t="s">
+        <v>271</v>
+      </c>
+      <c r="C71" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" t="s">
+        <v>272</v>
+      </c>
+      <c r="E71" t="s">
         <v>273</v>
       </c>
-      <c r="B71" t="s">
+      <c r="F71" t="s">
         <v>274</v>
-      </c>
-      <c r="C71" t="s">
-        <v>31</v>
-      </c>
-      <c r="D71" t="s">
-        <v>275</v>
-      </c>
-      <c r="E71" t="s">
-        <v>276</v>
-      </c>
-      <c r="F71" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>275</v>
+      </c>
+      <c r="B72" t="s">
+        <v>276</v>
+      </c>
+      <c r="C72" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" t="s">
+        <v>277</v>
+      </c>
+      <c r="E72" t="s">
         <v>278</v>
-      </c>
-      <c r="B72" t="s">
-        <v>279</v>
-      </c>
-      <c r="C72" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" t="s">
-        <v>280</v>
-      </c>
-      <c r="E72" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D73" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F73" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D74" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F74" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C75" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D75" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F75" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D76" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F76" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C77" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D77" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F77" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B78" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D78" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F78" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B79" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D79" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F79" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B80" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C80" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D80" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F80" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B81" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C81" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D81" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F81" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C82" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D82" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F82" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B83" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C83" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D83" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F83" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B84" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C84" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D84" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F84" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B85" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C85" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D85" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F85" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C86" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D86" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F86" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B87" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C87" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D87" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F87" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B88" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C88" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D88" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E88" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B89" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C89" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D89" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E89" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C90" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D90" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E90" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B91" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C91" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D91" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E91" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B92" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C92" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D92" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E92" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B93" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C93" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D93" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E93" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B94" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C94" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D94" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E94" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B95" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C95" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D95" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E95" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C96" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D96" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F96" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>336</v>
+      </c>
+      <c r="B97" t="s">
+        <v>150</v>
+      </c>
+      <c r="C97" t="s">
+        <v>337</v>
+      </c>
+      <c r="D97" t="s">
+        <v>338</v>
+      </c>
+      <c r="E97" t="s">
         <v>339</v>
-      </c>
-      <c r="B97" t="s">
-        <v>153</v>
-      </c>
-      <c r="C97" t="s">
-        <v>340</v>
-      </c>
-      <c r="D97" t="s">
-        <v>341</v>
-      </c>
-      <c r="E97" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B98" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C98" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D98" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E98" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B99" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C99" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D99" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E99" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F99" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B100" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C100" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D100" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E100" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C101" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D101" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E101" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B102" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C102" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D102" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E102" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C103" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D103" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E103" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C104" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D104" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E104" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel and role
</commit_message>
<xml_diff>
--- a/database/seeders/excel/user_niise_baru.xlsx
+++ b/database/seeders/excel/user_niise_baru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AFFD58-4843-4CEF-8C48-1285649A9E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20ACA81-E96D-400E-B8B1-619A0B015CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9578E655-562C-4104-B8F7-418F8D65ADB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{9578E655-562C-4104-B8F7-418F8D65ADB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="353">
   <si>
     <t>Jabatan Imigresen Malaysia Negeri Johor</t>
   </si>
@@ -1007,24 +1007,6 @@
     <t>jim3@heitech.com.my</t>
   </si>
   <si>
-    <t>NOC 1</t>
-  </si>
-  <si>
-    <t>noc1@heitech.com.my</t>
-  </si>
-  <si>
-    <t>noc3@heitech.com.my</t>
-  </si>
-  <si>
-    <t>noc2@heitech.com.my</t>
-  </si>
-  <si>
-    <t>NOC 2</t>
-  </si>
-  <si>
-    <t>NOC 3</t>
-  </si>
-  <si>
     <t>FrontLiner 1</t>
   </si>
   <si>
@@ -1098,6 +1080,21 @@
   </si>
   <si>
     <t>UTC KUCHING</t>
+  </si>
+  <si>
+    <t>BTMR</t>
+  </si>
+  <si>
+    <t>JIM</t>
+  </si>
+  <si>
+    <t>FRONTLINER</t>
+  </si>
+  <si>
+    <t>ICT_SV</t>
+  </si>
+  <si>
+    <t>CONTRACTOR</t>
   </si>
 </sst>
 </file>
@@ -1554,23 +1551,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C254406F-12FB-4ABC-BFDB-626D932D93E0}">
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C122"/>
+    <sheetView tabSelected="1" topLeftCell="B91" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+    <col min="3" max="3" width="75.88671875" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" customWidth="1"/>
+    <col min="5" max="5" width="34.44140625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1590,7 +1587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1610,7 +1607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1647,7 +1644,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1664,7 +1661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1684,7 +1681,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1704,7 +1701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1744,7 +1741,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1761,7 +1758,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1778,7 +1775,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1795,7 +1792,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -1812,7 +1809,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1829,7 +1826,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1846,7 +1843,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1886,7 +1883,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1906,7 +1903,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1914,7 +1911,7 @@
         <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D19" t="s">
         <v>75</v>
@@ -1923,7 +1920,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -1931,7 +1928,7 @@
         <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D20" t="s">
         <v>79</v>
@@ -1940,7 +1937,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1948,7 +1945,7 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D21" t="s">
         <v>82</v>
@@ -1960,7 +1957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1968,7 +1965,7 @@
         <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D22" t="s">
         <v>86</v>
@@ -1980,7 +1977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1988,7 +1985,7 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D23" t="s">
         <v>89</v>
@@ -1997,7 +1994,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -2005,7 +2002,7 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D24" t="s">
         <v>92</v>
@@ -2014,7 +2011,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2022,7 +2019,7 @@
         <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D25" t="s">
         <v>96</v>
@@ -2031,7 +2028,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2039,7 +2036,7 @@
         <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D26" t="s">
         <v>99</v>
@@ -2048,7 +2045,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -2056,7 +2053,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D27" t="s">
         <v>102</v>
@@ -2068,7 +2065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -2076,7 +2073,7 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D28" t="s">
         <v>105</v>
@@ -2088,7 +2085,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2096,7 +2093,7 @@
         <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D29" t="s">
         <v>110</v>
@@ -2105,7 +2102,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -2113,7 +2110,7 @@
         <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D30" t="s">
         <v>113</v>
@@ -2122,7 +2119,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>115</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D31" t="s">
         <v>116</v>
@@ -2142,7 +2139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -2150,7 +2147,7 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D32" t="s">
         <v>119</v>
@@ -2159,7 +2156,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -2167,7 +2164,7 @@
         <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D33" t="s">
         <v>122</v>
@@ -2176,7 +2173,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>124</v>
       </c>
@@ -2184,7 +2181,7 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D34" t="s">
         <v>125</v>
@@ -2196,7 +2193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>127</v>
       </c>
@@ -2204,7 +2201,7 @@
         <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D35" t="s">
         <v>128</v>
@@ -2216,7 +2213,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>130</v>
       </c>
@@ -2224,7 +2221,7 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D36" t="s">
         <v>131</v>
@@ -2233,7 +2230,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -2241,7 +2238,7 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D37" t="s">
         <v>134</v>
@@ -2250,7 +2247,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>127</v>
       </c>
@@ -2258,7 +2255,7 @@
         <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D38" t="s">
         <v>128</v>
@@ -2270,7 +2267,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>130</v>
       </c>
@@ -2278,7 +2275,7 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D39" t="s">
         <v>131</v>
@@ -2287,7 +2284,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -2295,7 +2292,7 @@
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D40" t="s">
         <v>134</v>
@@ -2304,7 +2301,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -2312,7 +2309,7 @@
         <v>137</v>
       </c>
       <c r="C41" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D41" t="s">
         <v>138</v>
@@ -2321,7 +2318,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>140</v>
       </c>
@@ -2329,7 +2326,7 @@
         <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D42" t="s">
         <v>141</v>
@@ -2338,7 +2335,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -2346,7 +2343,7 @@
         <v>144</v>
       </c>
       <c r="C43" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D43" t="s">
         <v>145</v>
@@ -2358,7 +2355,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -2366,7 +2363,7 @@
         <v>148</v>
       </c>
       <c r="C44" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D44" t="s">
         <v>149</v>
@@ -2375,7 +2372,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>151</v>
       </c>
@@ -2383,7 +2380,7 @@
         <v>74</v>
       </c>
       <c r="C45" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D45" t="s">
         <v>152</v>
@@ -2392,7 +2389,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>154</v>
       </c>
@@ -2400,7 +2397,7 @@
         <v>144</v>
       </c>
       <c r="C46" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D46" t="s">
         <v>155</v>
@@ -2412,7 +2409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>157</v>
       </c>
@@ -2420,7 +2417,7 @@
         <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D47" t="s">
         <v>158</v>
@@ -2429,7 +2426,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>160</v>
       </c>
@@ -2437,7 +2434,7 @@
         <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D48" t="s">
         <v>161</v>
@@ -2446,7 +2443,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>163</v>
       </c>
@@ -2454,7 +2451,7 @@
         <v>144</v>
       </c>
       <c r="C49" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D49" t="s">
         <v>164</v>
@@ -2466,7 +2463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>166</v>
       </c>
@@ -2474,7 +2471,7 @@
         <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D50" t="s">
         <v>167</v>
@@ -2483,7 +2480,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -2491,7 +2488,7 @@
         <v>137</v>
       </c>
       <c r="C51" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D51" t="s">
         <v>170</v>
@@ -2500,7 +2497,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>172</v>
       </c>
@@ -2508,7 +2505,7 @@
         <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D52" t="s">
         <v>173</v>
@@ -2520,7 +2517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>175</v>
       </c>
@@ -2528,7 +2525,7 @@
         <v>74</v>
       </c>
       <c r="C53" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D53" t="s">
         <v>176</v>
@@ -2537,7 +2534,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>178</v>
       </c>
@@ -2545,7 +2542,7 @@
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D54" t="s">
         <v>179</v>
@@ -2554,7 +2551,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>181</v>
       </c>
@@ -2562,7 +2559,7 @@
         <v>144</v>
       </c>
       <c r="C55" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D55" t="s">
         <v>182</v>
@@ -2571,7 +2568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>183</v>
       </c>
@@ -2579,7 +2576,7 @@
         <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D56" t="s">
         <v>184</v>
@@ -2588,7 +2585,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>186</v>
       </c>
@@ -2596,7 +2593,7 @@
         <v>74</v>
       </c>
       <c r="C57" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D57" t="s">
         <v>187</v>
@@ -2605,7 +2602,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>189</v>
       </c>
@@ -2613,7 +2610,7 @@
         <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D58" t="s">
         <v>190</v>
@@ -2625,7 +2622,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>191</v>
       </c>
@@ -2633,7 +2630,7 @@
         <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D59" t="s">
         <v>192</v>
@@ -2642,7 +2639,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>194</v>
       </c>
@@ -2650,7 +2647,7 @@
         <v>137</v>
       </c>
       <c r="C60" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D60" t="s">
         <v>195</v>
@@ -2659,7 +2656,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>197</v>
       </c>
@@ -2667,7 +2664,7 @@
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D61" t="s">
         <v>198</v>
@@ -2676,7 +2673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>199</v>
       </c>
@@ -2684,13 +2681,13 @@
         <v>85</v>
       </c>
       <c r="C62" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="F62" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>200</v>
       </c>
@@ -2698,7 +2695,7 @@
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D63" t="s">
         <v>201</v>
@@ -2707,7 +2704,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>203</v>
       </c>
@@ -2715,7 +2712,7 @@
         <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D64" t="s">
         <v>204</v>
@@ -2724,7 +2721,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>206</v>
       </c>
@@ -2732,7 +2729,7 @@
         <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D65" t="s">
         <v>207</v>
@@ -2741,7 +2738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>208</v>
       </c>
@@ -2749,7 +2746,7 @@
         <v>78</v>
       </c>
       <c r="C66" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D66" t="s">
         <v>209</v>
@@ -2758,7 +2755,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>211</v>
       </c>
@@ -2766,7 +2763,7 @@
         <v>78</v>
       </c>
       <c r="C67" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D67" t="s">
         <v>212</v>
@@ -2775,7 +2772,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>214</v>
       </c>
@@ -2783,7 +2780,7 @@
         <v>215</v>
       </c>
       <c r="C68" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D68" t="s">
         <v>216</v>
@@ -2795,7 +2792,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>219</v>
       </c>
@@ -2803,7 +2800,7 @@
         <v>220</v>
       </c>
       <c r="C69" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D69" t="s">
         <v>221</v>
@@ -2815,7 +2812,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>224</v>
       </c>
@@ -2823,7 +2820,7 @@
         <v>225</v>
       </c>
       <c r="C70" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D70" t="s">
         <v>226</v>
@@ -2835,7 +2832,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>229</v>
       </c>
@@ -2843,7 +2840,7 @@
         <v>230</v>
       </c>
       <c r="C71" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D71" t="s">
         <v>231</v>
@@ -2855,7 +2852,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>234</v>
       </c>
@@ -2863,7 +2860,7 @@
         <v>235</v>
       </c>
       <c r="C72" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D72" t="s">
         <v>236</v>
@@ -2872,7 +2869,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>238</v>
       </c>
@@ -2880,7 +2877,7 @@
         <v>20</v>
       </c>
       <c r="C73" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D73" t="s">
         <v>239</v>
@@ -2889,7 +2886,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>241</v>
       </c>
@@ -2897,7 +2894,7 @@
         <v>20</v>
       </c>
       <c r="C74" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D74" t="s">
         <v>242</v>
@@ -2906,7 +2903,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>243</v>
       </c>
@@ -2914,7 +2911,7 @@
         <v>20</v>
       </c>
       <c r="C75" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D75" t="s">
         <v>244</v>
@@ -2923,7 +2920,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>245</v>
       </c>
@@ -2931,7 +2928,7 @@
         <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D76" t="s">
         <v>246</v>
@@ -2940,7 +2937,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>247</v>
       </c>
@@ -2948,7 +2945,7 @@
         <v>20</v>
       </c>
       <c r="C77" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D77" t="s">
         <v>248</v>
@@ -2957,7 +2954,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>249</v>
       </c>
@@ -2965,7 +2962,7 @@
         <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D78" t="s">
         <v>250</v>
@@ -2974,7 +2971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>251</v>
       </c>
@@ -2982,7 +2979,7 @@
         <v>20</v>
       </c>
       <c r="C79" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D79" t="s">
         <v>252</v>
@@ -2991,7 +2988,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>253</v>
       </c>
@@ -2999,7 +2996,7 @@
         <v>20</v>
       </c>
       <c r="C80" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D80" t="s">
         <v>254</v>
@@ -3008,7 +3005,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>255</v>
       </c>
@@ -3016,7 +3013,7 @@
         <v>20</v>
       </c>
       <c r="C81" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D81" t="s">
         <v>256</v>
@@ -3025,7 +3022,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>257</v>
       </c>
@@ -3033,7 +3030,7 @@
         <v>20</v>
       </c>
       <c r="C82" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D82" t="s">
         <v>258</v>
@@ -3042,7 +3039,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>259</v>
       </c>
@@ -3050,7 +3047,7 @@
         <v>20</v>
       </c>
       <c r="C83" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D83" t="s">
         <v>260</v>
@@ -3059,7 +3056,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>261</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>20</v>
       </c>
       <c r="C84" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D84" t="s">
         <v>262</v>
@@ -3076,7 +3073,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>263</v>
       </c>
@@ -3084,7 +3081,7 @@
         <v>20</v>
       </c>
       <c r="C85" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D85" t="s">
         <v>264</v>
@@ -3093,7 +3090,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>265</v>
       </c>
@@ -3101,7 +3098,7 @@
         <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D86" t="s">
         <v>266</v>
@@ -3110,7 +3107,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>267</v>
       </c>
@@ -3118,7 +3115,7 @@
         <v>20</v>
       </c>
       <c r="C87" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D87" t="s">
         <v>268</v>
@@ -3127,7 +3124,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>269</v>
       </c>
@@ -3135,7 +3132,7 @@
         <v>28</v>
       </c>
       <c r="C88" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D88" t="s">
         <v>270</v>
@@ -3144,7 +3141,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>272</v>
       </c>
@@ -3152,7 +3149,7 @@
         <v>109</v>
       </c>
       <c r="C89" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D89" t="s">
         <v>273</v>
@@ -3161,7 +3158,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>275</v>
       </c>
@@ -3169,7 +3166,7 @@
         <v>78</v>
       </c>
       <c r="C90" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D90" t="s">
         <v>276</v>
@@ -3178,7 +3175,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>278</v>
       </c>
@@ -3186,7 +3183,7 @@
         <v>74</v>
       </c>
       <c r="C91" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D91" t="s">
         <v>279</v>
@@ -3195,7 +3192,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>281</v>
       </c>
@@ -3203,7 +3200,7 @@
         <v>74</v>
       </c>
       <c r="C92" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D92" t="s">
         <v>282</v>
@@ -3212,7 +3209,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>284</v>
       </c>
@@ -3220,7 +3217,7 @@
         <v>78</v>
       </c>
       <c r="C93" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D93" t="s">
         <v>285</v>
@@ -3229,7 +3226,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>287</v>
       </c>
@@ -3237,7 +3234,7 @@
         <v>109</v>
       </c>
       <c r="C94" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D94" t="s">
         <v>288</v>
@@ -3246,7 +3243,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>290</v>
       </c>
@@ -3254,7 +3251,7 @@
         <v>109</v>
       </c>
       <c r="C95" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D95" t="s">
         <v>291</v>
@@ -3263,7 +3260,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>293</v>
       </c>
@@ -3271,7 +3268,7 @@
         <v>144</v>
       </c>
       <c r="C96" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D96" t="s">
         <v>294</v>
@@ -3280,7 +3277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>295</v>
       </c>
@@ -3288,7 +3285,7 @@
         <v>109</v>
       </c>
       <c r="C97" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D97" t="s">
         <v>296</v>
@@ -3297,7 +3294,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>298</v>
       </c>
@@ -3305,7 +3302,7 @@
         <v>109</v>
       </c>
       <c r="C98" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D98" t="s">
         <v>299</v>
@@ -3314,7 +3311,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>301</v>
       </c>
@@ -3322,7 +3319,7 @@
         <v>144</v>
       </c>
       <c r="C99" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D99" t="s">
         <v>302</v>
@@ -3334,7 +3331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -3342,7 +3339,7 @@
         <v>78</v>
       </c>
       <c r="C100" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D100" t="s">
         <v>305</v>
@@ -3351,7 +3348,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -3359,7 +3356,7 @@
         <v>74</v>
       </c>
       <c r="C101" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D101" t="s">
         <v>308</v>
@@ -3368,7 +3365,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>310</v>
       </c>
@@ -3376,7 +3373,7 @@
         <v>74</v>
       </c>
       <c r="C102" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D102" t="s">
         <v>311</v>
@@ -3384,11 +3381,11 @@
       <c r="E102" t="s">
         <v>309</v>
       </c>
-      <c r="G102">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>312</v>
       </c>
@@ -3396,7 +3393,7 @@
         <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D103" t="s">
         <v>313</v>
@@ -3404,11 +3401,11 @@
       <c r="E103" t="s">
         <v>309</v>
       </c>
-      <c r="G103">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>314</v>
       </c>
@@ -3416,7 +3413,7 @@
         <v>74</v>
       </c>
       <c r="C104" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D104" t="s">
         <v>315</v>
@@ -3424,11 +3421,11 @@
       <c r="E104" t="s">
         <v>309</v>
       </c>
-      <c r="G104">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>318</v>
       </c>
@@ -3436,7 +3433,7 @@
         <v>74</v>
       </c>
       <c r="C105" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>317</v>
@@ -3444,11 +3441,11 @@
       <c r="E105" t="s">
         <v>309</v>
       </c>
-      <c r="G105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>319</v>
       </c>
@@ -3456,7 +3453,7 @@
         <v>74</v>
       </c>
       <c r="C106" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>320</v>
@@ -3464,11 +3461,11 @@
       <c r="E106" t="s">
         <v>309</v>
       </c>
-      <c r="G106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>321</v>
       </c>
@@ -3476,7 +3473,7 @@
         <v>74</v>
       </c>
       <c r="C107" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>322</v>
@@ -3484,11 +3481,11 @@
       <c r="E107" t="s">
         <v>309</v>
       </c>
-      <c r="G107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>323</v>
       </c>
@@ -3496,179 +3493,179 @@
         <v>74</v>
       </c>
       <c r="C108" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E108" t="s">
         <v>309</v>
       </c>
-      <c r="G108">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B109" t="s">
         <v>74</v>
       </c>
       <c r="C109" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E109" t="s">
         <v>309</v>
       </c>
-      <c r="G109">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B110" t="s">
         <v>74</v>
       </c>
       <c r="C110" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="E110" t="s">
         <v>309</v>
       </c>
-      <c r="G110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B111" t="s">
         <v>74</v>
       </c>
       <c r="C111" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E111" t="s">
         <v>309</v>
       </c>
-      <c r="G111">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B112" t="s">
         <v>74</v>
       </c>
       <c r="C112" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E112" t="s">
         <v>309</v>
       </c>
-      <c r="G112">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B113" t="s">
         <v>74</v>
       </c>
       <c r="C113" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E113" t="s">
         <v>309</v>
       </c>
-      <c r="G113">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B114" t="s">
         <v>74</v>
       </c>
       <c r="C114" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E114" t="s">
         <v>309</v>
       </c>
-      <c r="G114">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G114" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B115" t="s">
         <v>74</v>
       </c>
       <c r="C115" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E115" t="s">
         <v>309</v>
       </c>
-      <c r="G115">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B116" t="s">
         <v>74</v>
       </c>
       <c r="C116" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E116" t="s">
         <v>309</v>
       </c>
-      <c r="G116">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G116" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>341</v>
       </c>
@@ -3676,19 +3673,19 @@
         <v>74</v>
       </c>
       <c r="C117" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E117" t="s">
         <v>309</v>
       </c>
-      <c r="G117">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G117" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>342</v>
       </c>
@@ -3696,7 +3693,7 @@
         <v>74</v>
       </c>
       <c r="C118" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>345</v>
@@ -3704,11 +3701,11 @@
       <c r="E118" t="s">
         <v>309</v>
       </c>
-      <c r="G118">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G118" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>343</v>
       </c>
@@ -3716,76 +3713,16 @@
         <v>74</v>
       </c>
       <c r="C119" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E119" t="s">
         <v>309</v>
       </c>
-      <c r="G119">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>347</v>
-      </c>
-      <c r="B120" t="s">
-        <v>74</v>
-      </c>
-      <c r="C120" t="s">
-        <v>353</v>
-      </c>
-      <c r="D120" s="9" t="s">
+      <c r="G119" t="s">
         <v>352</v>
-      </c>
-      <c r="E120" t="s">
-        <v>309</v>
-      </c>
-      <c r="G120">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>348</v>
-      </c>
-      <c r="B121" t="s">
-        <v>74</v>
-      </c>
-      <c r="C121" t="s">
-        <v>353</v>
-      </c>
-      <c r="D121" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="E121" t="s">
-        <v>309</v>
-      </c>
-      <c r="G121">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>349</v>
-      </c>
-      <c r="B122" t="s">
-        <v>74</v>
-      </c>
-      <c r="C122" t="s">
-        <v>353</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="E122" t="s">
-        <v>309</v>
-      </c>
-      <c r="G122">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3793,21 +3730,18 @@
     <hyperlink ref="D105" r:id="rId1" xr:uid="{38C8D6B3-2A28-4B0D-971D-B439FF5F161B}"/>
     <hyperlink ref="D106" r:id="rId2" xr:uid="{D546F8A5-BDA2-4371-AE09-1FE7930F7B56}"/>
     <hyperlink ref="D107" r:id="rId3" xr:uid="{7D8B0B13-BB99-47BE-8A58-369C0FAAA8F0}"/>
-    <hyperlink ref="D108" r:id="rId4" xr:uid="{5FE5B157-81E9-4092-A2EA-2F078452EF1D}"/>
-    <hyperlink ref="D109" r:id="rId5" xr:uid="{3CD52F81-D227-4CB4-9304-3817DAADB4E7}"/>
-    <hyperlink ref="D110" r:id="rId6" xr:uid="{0A046500-35C4-470A-8423-D4FF5EE3F3FA}"/>
-    <hyperlink ref="D111" r:id="rId7" xr:uid="{2ACE40EE-F32B-469E-9138-18CC93E58341}"/>
-    <hyperlink ref="D112" r:id="rId8" xr:uid="{85611653-0A42-42FA-8EA8-83ACA36634C4}"/>
-    <hyperlink ref="D113" r:id="rId9" xr:uid="{3F2EDF05-2AA6-48CA-8571-05996DBDF04B}"/>
-    <hyperlink ref="D114" r:id="rId10" xr:uid="{1AE302C8-C6C0-4D88-86A3-79700788E544}"/>
-    <hyperlink ref="D115" r:id="rId11" xr:uid="{E2F6B6E8-702A-46D1-83F4-6D59AF6F717B}"/>
-    <hyperlink ref="D116" r:id="rId12" xr:uid="{A09B6AA3-64CD-4AE0-9FAC-B9E8EF186E1B}"/>
-    <hyperlink ref="D117" r:id="rId13" xr:uid="{82BE7B6B-F7A8-4A65-9DE9-B15B890DBBA6}"/>
-    <hyperlink ref="D118" r:id="rId14" xr:uid="{A922F855-F1FF-4681-AFBD-70E0CE5EFFF7}"/>
-    <hyperlink ref="D119" r:id="rId15" xr:uid="{9B5060A5-1798-47ED-9C4D-C842FFC1DD20}"/>
-    <hyperlink ref="D120" r:id="rId16" xr:uid="{B5FE88D1-AFC5-46D6-B9A1-23AE866065B9}"/>
-    <hyperlink ref="D121" r:id="rId17" xr:uid="{F24BB39F-58DA-4536-B093-20394EB572F9}"/>
-    <hyperlink ref="D122" r:id="rId18" xr:uid="{26762B9C-6E99-4BBA-8DD7-E37BFDFB4A5D}"/>
+    <hyperlink ref="D108" r:id="rId4" xr:uid="{2ACE40EE-F32B-469E-9138-18CC93E58341}"/>
+    <hyperlink ref="D109" r:id="rId5" xr:uid="{85611653-0A42-42FA-8EA8-83ACA36634C4}"/>
+    <hyperlink ref="D110" r:id="rId6" xr:uid="{3F2EDF05-2AA6-48CA-8571-05996DBDF04B}"/>
+    <hyperlink ref="D111" r:id="rId7" xr:uid="{1AE302C8-C6C0-4D88-86A3-79700788E544}"/>
+    <hyperlink ref="D112" r:id="rId8" xr:uid="{E2F6B6E8-702A-46D1-83F4-6D59AF6F717B}"/>
+    <hyperlink ref="D113" r:id="rId9" xr:uid="{A09B6AA3-64CD-4AE0-9FAC-B9E8EF186E1B}"/>
+    <hyperlink ref="D114" r:id="rId10" xr:uid="{82BE7B6B-F7A8-4A65-9DE9-B15B890DBBA6}"/>
+    <hyperlink ref="D115" r:id="rId11" xr:uid="{A922F855-F1FF-4681-AFBD-70E0CE5EFFF7}"/>
+    <hyperlink ref="D116" r:id="rId12" xr:uid="{9B5060A5-1798-47ED-9C4D-C842FFC1DD20}"/>
+    <hyperlink ref="D117" r:id="rId13" xr:uid="{B5FE88D1-AFC5-46D6-B9A1-23AE866065B9}"/>
+    <hyperlink ref="D118" r:id="rId14" xr:uid="{F24BB39F-58DA-4536-B093-20394EB572F9}"/>
+    <hyperlink ref="D119" r:id="rId15" xr:uid="{26762B9C-6E99-4BBA-8DD7-E37BFDFB4A5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update excel user and seeder
</commit_message>
<xml_diff>
--- a/database/seeders/excel/user_niise_baru.xlsx
+++ b/database/seeders/excel/user_niise_baru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20ACA81-E96D-400E-B8B1-619A0B015CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9BFBFB-F188-4517-8FB4-263BE5E37EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{9578E655-562C-4104-B8F7-418F8D65ADB7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="353">
   <si>
     <t>Jabatan Imigresen Malaysia Negeri Johor</t>
   </si>
@@ -1551,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C254406F-12FB-4ABC-BFDB-626D932D93E0}">
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B91" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2195,27 +2195,24 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
         <v>347</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E35" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
         <v>28</v>
@@ -2224,52 +2221,52 @@
         <v>347</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
         <v>347</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>129</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
         <v>347</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E38" t="s">
-        <v>129</v>
-      </c>
-      <c r="F38" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
@@ -2278,32 +2275,32 @@
         <v>347</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E39" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="C40" t="s">
         <v>347</v>
       </c>
       <c r="D40" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E40" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
         <v>137</v>
@@ -2312,106 +2309,106 @@
         <v>347</v>
       </c>
       <c r="D41" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
         <v>347</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>146</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>347</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
-      </c>
-      <c r="F43" t="s">
-        <v>13</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
         <v>347</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E44" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="C45" t="s">
         <v>347</v>
       </c>
       <c r="D45" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E45" t="s">
-        <v>153</v>
+        <v>156</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
         <v>347</v>
       </c>
       <c r="D46" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E46" t="s">
-        <v>156</v>
-      </c>
-      <c r="F46" t="s">
-        <v>13</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B47" t="s">
         <v>78</v>
@@ -2420,106 +2417,106 @@
         <v>347</v>
       </c>
       <c r="D47" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="C48" t="s">
         <v>347</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>165</v>
+      </c>
+      <c r="F48" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>163</v>
-      </c>
-      <c r="B49" t="s">
-        <v>144</v>
+        <v>166</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C49" t="s">
         <v>347</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E49" t="s">
-        <v>165</v>
-      </c>
-      <c r="F49" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>166</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>74</v>
+        <v>169</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C50" t="s">
         <v>347</v>
       </c>
       <c r="D50" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E50" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
         <v>347</v>
       </c>
       <c r="D51" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E51" t="s">
-        <v>171</v>
+        <v>174</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C52" t="s">
         <v>347</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
-      </c>
-      <c r="F52" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>74</v>
@@ -2528,219 +2525,219 @@
         <v>347</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E53" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="C54" t="s">
         <v>347</v>
       </c>
       <c r="D54" t="s">
-        <v>179</v>
-      </c>
-      <c r="E54" t="s">
-        <v>180</v>
+        <v>182</v>
+      </c>
+      <c r="F54" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="C55" t="s">
         <v>347</v>
       </c>
       <c r="D55" t="s">
-        <v>182</v>
-      </c>
-      <c r="F55" t="s">
-        <v>13</v>
+        <v>184</v>
+      </c>
+      <c r="E55" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>183</v>
-      </c>
-      <c r="B56" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C56" t="s">
         <v>347</v>
       </c>
       <c r="D56" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E56" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>186</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>74</v>
+        <v>189</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
       </c>
       <c r="C57" t="s">
         <v>347</v>
       </c>
       <c r="D57" t="s">
-        <v>187</v>
-      </c>
-      <c r="E57" t="s">
-        <v>188</v>
+        <v>190</v>
+      </c>
+      <c r="F57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>189</v>
-      </c>
-      <c r="B58" t="s">
-        <v>10</v>
+        <v>191</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="C58" t="s">
         <v>347</v>
       </c>
       <c r="D58" t="s">
-        <v>190</v>
-      </c>
-      <c r="F58" t="s">
-        <v>13</v>
-      </c>
-      <c r="J58" t="s">
-        <v>316</v>
+        <v>192</v>
+      </c>
+      <c r="E58" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>191</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>109</v>
+        <v>194</v>
+      </c>
+      <c r="B59" t="s">
+        <v>137</v>
       </c>
       <c r="C59" t="s">
         <v>347</v>
       </c>
       <c r="D59" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E59" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="C60" t="s">
         <v>347</v>
       </c>
       <c r="D60" t="s">
-        <v>195</v>
-      </c>
-      <c r="E60" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="F60" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C61" t="s">
         <v>347</v>
       </c>
-      <c r="D61" t="s">
-        <v>198</v>
-      </c>
       <c r="F61" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="C62" t="s">
         <v>347</v>
       </c>
-      <c r="F62" t="s">
-        <v>107</v>
+      <c r="D62" t="s">
+        <v>201</v>
+      </c>
+      <c r="E62" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B63" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="C63" t="s">
         <v>347</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E63" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
         <v>347</v>
       </c>
       <c r="D64" t="s">
-        <v>204</v>
-      </c>
-      <c r="E64" t="s">
-        <v>205</v>
+        <v>207</v>
+      </c>
+      <c r="F64" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C65" t="s">
         <v>347</v>
       </c>
       <c r="D65" t="s">
-        <v>207</v>
-      </c>
-      <c r="F65" t="s">
-        <v>13</v>
+        <v>209</v>
+      </c>
+      <c r="E65" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B66" t="s">
         <v>78</v>
@@ -2749,129 +2746,129 @@
         <v>347</v>
       </c>
       <c r="D66" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E66" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>215</v>
       </c>
       <c r="C67" t="s">
         <v>347</v>
       </c>
       <c r="D67" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E67" t="s">
-        <v>213</v>
+        <v>217</v>
+      </c>
+      <c r="F67" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B68" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C68" t="s">
         <v>347</v>
       </c>
       <c r="D68" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E68" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F68" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B69" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C69" t="s">
         <v>347</v>
       </c>
       <c r="D69" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E69" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F69" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B70" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C70" t="s">
         <v>347</v>
       </c>
       <c r="D70" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E70" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F70" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B71" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C71" t="s">
         <v>347</v>
       </c>
       <c r="D71" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E71" t="s">
-        <v>232</v>
-      </c>
-      <c r="F71" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B72" t="s">
-        <v>235</v>
+        <v>20</v>
       </c>
       <c r="C72" t="s">
         <v>347</v>
       </c>
       <c r="D72" t="s">
-        <v>236</v>
-      </c>
-      <c r="E72" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="F72" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B73" t="s">
         <v>20</v>
@@ -2880,7 +2877,7 @@
         <v>347</v>
       </c>
       <c r="D73" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F73" t="s">
         <v>240</v>
@@ -2888,7 +2885,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B74" t="s">
         <v>20</v>
@@ -2897,7 +2894,7 @@
         <v>347</v>
       </c>
       <c r="D74" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F74" t="s">
         <v>240</v>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B75" t="s">
         <v>20</v>
@@ -2914,7 +2911,7 @@
         <v>347</v>
       </c>
       <c r="D75" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F75" t="s">
         <v>240</v>
@@ -2922,7 +2919,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B76" t="s">
         <v>20</v>
@@ -2931,7 +2928,7 @@
         <v>347</v>
       </c>
       <c r="D76" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F76" t="s">
         <v>240</v>
@@ -2939,7 +2936,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B77" t="s">
         <v>20</v>
@@ -2948,15 +2945,15 @@
         <v>347</v>
       </c>
       <c r="D77" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F77" t="s">
-        <v>240</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B78" t="s">
         <v>20</v>
@@ -2965,15 +2962,15 @@
         <v>347</v>
       </c>
       <c r="D78" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F78" t="s">
-        <v>36</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B79" t="s">
         <v>20</v>
@@ -2982,7 +2979,7 @@
         <v>347</v>
       </c>
       <c r="D79" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F79" t="s">
         <v>240</v>
@@ -2990,7 +2987,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B80" t="s">
         <v>20</v>
@@ -2999,7 +2996,7 @@
         <v>347</v>
       </c>
       <c r="D80" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F80" t="s">
         <v>240</v>
@@ -3007,7 +3004,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B81" t="s">
         <v>20</v>
@@ -3016,7 +3013,7 @@
         <v>347</v>
       </c>
       <c r="D81" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F81" t="s">
         <v>240</v>
@@ -3024,7 +3021,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B82" t="s">
         <v>20</v>
@@ -3033,7 +3030,7 @@
         <v>347</v>
       </c>
       <c r="D82" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F82" t="s">
         <v>240</v>
@@ -3041,7 +3038,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B83" t="s">
         <v>20</v>
@@ -3050,7 +3047,7 @@
         <v>347</v>
       </c>
       <c r="D83" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F83" t="s">
         <v>240</v>
@@ -3058,7 +3055,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B84" t="s">
         <v>20</v>
@@ -3067,7 +3064,7 @@
         <v>347</v>
       </c>
       <c r="D84" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F84" t="s">
         <v>240</v>
@@ -3075,7 +3072,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B85" t="s">
         <v>20</v>
@@ -3084,7 +3081,7 @@
         <v>347</v>
       </c>
       <c r="D85" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F85" t="s">
         <v>240</v>
@@ -3092,7 +3089,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B86" t="s">
         <v>20</v>
@@ -3101,83 +3098,83 @@
         <v>347</v>
       </c>
       <c r="D86" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F86" t="s">
-        <v>240</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C87" t="s">
         <v>347</v>
       </c>
       <c r="D87" t="s">
-        <v>268</v>
-      </c>
-      <c r="F87" t="s">
-        <v>36</v>
+        <v>270</v>
+      </c>
+      <c r="E87" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B88" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="C88" t="s">
         <v>347</v>
       </c>
       <c r="D88" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E88" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B89" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C89" t="s">
         <v>347</v>
       </c>
       <c r="D89" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E89" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C90" t="s">
         <v>347</v>
       </c>
       <c r="D90" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E90" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B91" t="s">
         <v>74</v>
@@ -3186,49 +3183,49 @@
         <v>347</v>
       </c>
       <c r="D91" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E91" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B92" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C92" t="s">
         <v>347</v>
       </c>
       <c r="D92" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E92" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B93" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C93" t="s">
         <v>347</v>
       </c>
       <c r="D93" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E93" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B94" t="s">
         <v>109</v>
@@ -3237,49 +3234,49 @@
         <v>347</v>
       </c>
       <c r="D94" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E94" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="C95" t="s">
         <v>347</v>
       </c>
       <c r="D95" t="s">
-        <v>291</v>
-      </c>
-      <c r="E95" t="s">
-        <v>292</v>
+        <v>294</v>
+      </c>
+      <c r="F95" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B96" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="C96" t="s">
         <v>347</v>
       </c>
       <c r="D96" t="s">
-        <v>294</v>
-      </c>
-      <c r="F96" t="s">
-        <v>13</v>
+        <v>296</v>
+      </c>
+      <c r="E96" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B97" t="s">
         <v>109</v>
@@ -3288,69 +3285,69 @@
         <v>347</v>
       </c>
       <c r="D97" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="E97" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B98" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="C98" t="s">
         <v>347</v>
       </c>
       <c r="D98" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E98" t="s">
-        <v>300</v>
+        <v>303</v>
+      </c>
+      <c r="F98" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B99" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
       <c r="C99" t="s">
         <v>347</v>
       </c>
       <c r="D99" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E99" t="s">
-        <v>303</v>
-      </c>
-      <c r="F99" t="s">
-        <v>13</v>
+        <v>306</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B100" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C100" t="s">
         <v>347</v>
       </c>
       <c r="D100" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E100" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B101" t="s">
         <v>74</v>
@@ -3359,15 +3356,18 @@
         <v>347</v>
       </c>
       <c r="D101" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E101" t="s">
         <v>309</v>
       </c>
+      <c r="G101" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B102" t="s">
         <v>74</v>
@@ -3376,7 +3376,7 @@
         <v>347</v>
       </c>
       <c r="D102" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E102" t="s">
         <v>309</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B103" t="s">
         <v>74</v>
@@ -3396,7 +3396,7 @@
         <v>347</v>
       </c>
       <c r="D103" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E103" t="s">
         <v>309</v>
@@ -3407,7 +3407,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B104" t="s">
         <v>74</v>
@@ -3415,19 +3415,19 @@
       <c r="C104" t="s">
         <v>347</v>
       </c>
-      <c r="D104" t="s">
-        <v>315</v>
+      <c r="D104" s="9" t="s">
+        <v>317</v>
       </c>
       <c r="E104" t="s">
         <v>309</v>
       </c>
       <c r="G104" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B105" t="s">
         <v>74</v>
@@ -3436,7 +3436,7 @@
         <v>347</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E105" t="s">
         <v>309</v>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B106" t="s">
         <v>74</v>
@@ -3456,7 +3456,7 @@
         <v>347</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E106" t="s">
         <v>309</v>
@@ -3467,7 +3467,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B107" t="s">
         <v>74</v>
@@ -3476,18 +3476,18 @@
         <v>347</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="E107" t="s">
         <v>309</v>
       </c>
       <c r="G107" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B108" t="s">
         <v>74</v>
@@ -3496,7 +3496,7 @@
         <v>347</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E108" t="s">
         <v>309</v>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B109" t="s">
         <v>74</v>
@@ -3516,7 +3516,7 @@
         <v>347</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="E109" t="s">
         <v>309</v>
@@ -3527,7 +3527,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B110" t="s">
         <v>74</v>
@@ -3536,18 +3536,18 @@
         <v>347</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E110" t="s">
         <v>309</v>
       </c>
       <c r="G110" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B111" t="s">
         <v>74</v>
@@ -3556,7 +3556,7 @@
         <v>347</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E111" t="s">
         <v>309</v>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B112" t="s">
         <v>74</v>
@@ -3576,7 +3576,7 @@
         <v>347</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E112" t="s">
         <v>309</v>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="B113" t="s">
         <v>74</v>
@@ -3596,18 +3596,18 @@
         <v>347</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="E113" t="s">
         <v>309</v>
       </c>
       <c r="G113" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B114" t="s">
         <v>74</v>
@@ -3616,7 +3616,7 @@
         <v>347</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E114" t="s">
         <v>309</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B115" t="s">
         <v>74</v>
@@ -3636,7 +3636,7 @@
         <v>347</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E115" t="s">
         <v>309</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B116" t="s">
         <v>74</v>
@@ -3656,18 +3656,18 @@
         <v>347</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="E116" t="s">
         <v>309</v>
       </c>
       <c r="G116" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B117" t="s">
         <v>74</v>
@@ -3676,7 +3676,7 @@
         <v>347</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E117" t="s">
         <v>309</v>
@@ -3687,7 +3687,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B118" t="s">
         <v>74</v>
@@ -3696,7 +3696,7 @@
         <v>347</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E118" t="s">
         <v>309</v>
@@ -3705,43 +3705,23 @@
         <v>352</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>343</v>
-      </c>
-      <c r="B119" t="s">
-        <v>74</v>
-      </c>
-      <c r="C119" t="s">
-        <v>347</v>
-      </c>
-      <c r="D119" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="E119" t="s">
-        <v>309</v>
-      </c>
-      <c r="G119" t="s">
-        <v>352</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D105" r:id="rId1" xr:uid="{38C8D6B3-2A28-4B0D-971D-B439FF5F161B}"/>
-    <hyperlink ref="D106" r:id="rId2" xr:uid="{D546F8A5-BDA2-4371-AE09-1FE7930F7B56}"/>
-    <hyperlink ref="D107" r:id="rId3" xr:uid="{7D8B0B13-BB99-47BE-8A58-369C0FAAA8F0}"/>
-    <hyperlink ref="D108" r:id="rId4" xr:uid="{2ACE40EE-F32B-469E-9138-18CC93E58341}"/>
-    <hyperlink ref="D109" r:id="rId5" xr:uid="{85611653-0A42-42FA-8EA8-83ACA36634C4}"/>
-    <hyperlink ref="D110" r:id="rId6" xr:uid="{3F2EDF05-2AA6-48CA-8571-05996DBDF04B}"/>
-    <hyperlink ref="D111" r:id="rId7" xr:uid="{1AE302C8-C6C0-4D88-86A3-79700788E544}"/>
-    <hyperlink ref="D112" r:id="rId8" xr:uid="{E2F6B6E8-702A-46D1-83F4-6D59AF6F717B}"/>
-    <hyperlink ref="D113" r:id="rId9" xr:uid="{A09B6AA3-64CD-4AE0-9FAC-B9E8EF186E1B}"/>
-    <hyperlink ref="D114" r:id="rId10" xr:uid="{82BE7B6B-F7A8-4A65-9DE9-B15B890DBBA6}"/>
-    <hyperlink ref="D115" r:id="rId11" xr:uid="{A922F855-F1FF-4681-AFBD-70E0CE5EFFF7}"/>
-    <hyperlink ref="D116" r:id="rId12" xr:uid="{9B5060A5-1798-47ED-9C4D-C842FFC1DD20}"/>
-    <hyperlink ref="D117" r:id="rId13" xr:uid="{B5FE88D1-AFC5-46D6-B9A1-23AE866065B9}"/>
-    <hyperlink ref="D118" r:id="rId14" xr:uid="{F24BB39F-58DA-4536-B093-20394EB572F9}"/>
-    <hyperlink ref="D119" r:id="rId15" xr:uid="{26762B9C-6E99-4BBA-8DD7-E37BFDFB4A5D}"/>
+    <hyperlink ref="D104" r:id="rId1" xr:uid="{38C8D6B3-2A28-4B0D-971D-B439FF5F161B}"/>
+    <hyperlink ref="D105" r:id="rId2" xr:uid="{D546F8A5-BDA2-4371-AE09-1FE7930F7B56}"/>
+    <hyperlink ref="D106" r:id="rId3" xr:uid="{7D8B0B13-BB99-47BE-8A58-369C0FAAA8F0}"/>
+    <hyperlink ref="D107" r:id="rId4" xr:uid="{2ACE40EE-F32B-469E-9138-18CC93E58341}"/>
+    <hyperlink ref="D108" r:id="rId5" xr:uid="{85611653-0A42-42FA-8EA8-83ACA36634C4}"/>
+    <hyperlink ref="D109" r:id="rId6" xr:uid="{3F2EDF05-2AA6-48CA-8571-05996DBDF04B}"/>
+    <hyperlink ref="D110" r:id="rId7" xr:uid="{1AE302C8-C6C0-4D88-86A3-79700788E544}"/>
+    <hyperlink ref="D111" r:id="rId8" xr:uid="{E2F6B6E8-702A-46D1-83F4-6D59AF6F717B}"/>
+    <hyperlink ref="D112" r:id="rId9" xr:uid="{A09B6AA3-64CD-4AE0-9FAC-B9E8EF186E1B}"/>
+    <hyperlink ref="D113" r:id="rId10" xr:uid="{82BE7B6B-F7A8-4A65-9DE9-B15B890DBBA6}"/>
+    <hyperlink ref="D114" r:id="rId11" xr:uid="{A922F855-F1FF-4681-AFBD-70E0CE5EFFF7}"/>
+    <hyperlink ref="D115" r:id="rId12" xr:uid="{9B5060A5-1798-47ED-9C4D-C842FFC1DD20}"/>
+    <hyperlink ref="D116" r:id="rId13" xr:uid="{B5FE88D1-AFC5-46D6-B9A1-23AE866065B9}"/>
+    <hyperlink ref="D117" r:id="rId14" xr:uid="{F24BB39F-58DA-4536-B093-20394EB572F9}"/>
+    <hyperlink ref="D118" r:id="rId15" xr:uid="{26762B9C-6E99-4BBA-8DD7-E37BFDFB4A5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>